<commit_message>
Stage2: ShenFri add A7 to A20
</commit_message>
<xml_diff>
--- a/ShenFri/evidence.xlsx
+++ b/ShenFri/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17280" windowHeight="16220" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView windowWidth="17280" windowHeight="7280" tabRatio="500" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120">
   <si>
     <t>TeamName</t>
   </si>
@@ -100,6 +100,12 @@
     <t>goniriscollectionid1</t>
   </si>
   <si>
+    <t>BE0B6F7B0716031F4249C1FA2CBBC488C3FE0C5ECB4C78731EB328D578E5E742</t>
+  </si>
+  <si>
+    <t>gonDenom</t>
+  </si>
+  <si>
     <t>NFTID</t>
   </si>
   <si>
@@ -115,6 +121,12 @@
     <t>gonirisnftid22</t>
   </si>
   <si>
+    <t>6D7A37F2F94DA54734039A60C334E6A2BFCCD629D235694C95F64A4074F791F0</t>
+  </si>
+  <si>
+    <t>nftId</t>
+  </si>
+  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -145,19 +157,241 @@
     <t>ibc/3DF9E9559818ED497EB1ED304E6FD24E8AFDEEAECDE7473614E4405BB16D8B6F</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
+    <t>stars130df8wpnq09ztljra7g0cpcnmqt69rerju5j65eqf5pvu6qgxd6s85r6ky</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; s --(1)--&gt; j --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>juno1lzhjrtx7guehr4sk258qptm9shv95g4s7lrz3wv5zhykh688yp9qdj0l0z</t>
+  </si>
+  <si>
+    <t>ibc/C7947865F3E9092C8B542E3E36004C642C27E4E56DDB1B240CE6089789270ED9</t>
+  </si>
+  <si>
+    <t>ibc/FFD2B0E45CC1E5AADB76CF0B4E90E46C7064A1405CEA719DCE1572BE7E0FD931</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; u --(1)--&gt; o --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>ibc/F6EE16141088F773ED0CD0C25632C4314D0ACAB3196FB732976993DB0DD5FCFD</t>
+  </si>
+  <si>
+    <t> ibc/3EF4792F7E2FFB8FBE5599B06F7D0DB6008EE62041D966BB7535B3913FA3B4B1</t>
+  </si>
+  <si>
+    <t>stars10ga4flzu8nmvdkvw62nfp04py27yysl5ap9fcwlaly5p7uyskytqpcj9xf</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; s --(1)--&gt; j --(1)--&gt; u --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>juno1h0mlwphdvqd9ceaeclrl527uujlyr3cahw2aleafr698kgw4g54qqzx0x4</t>
+  </si>
+  <si>
+    <t>ibc/CBA7E40E421589ACABE1BC629AA4E04F4DF45E79132E77B7282B108AD13BA456</t>
+  </si>
+  <si>
+    <t>ibc/BE8C4D1DAFD7CBDA7531701F7A1A57BBC04D4CBFFF4720EE7CEB1C9B28476195</t>
+  </si>
+  <si>
+    <t>stars17vqnsx2qm6f5mqev4mptgdfg3g0p535t784zev8qz2ukwdlps3jq3ts4jl</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; s --(1)--&gt; o --(1)--&gt; j --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>ibc/C23E35963AF88C873C901D9F8E70994C6C2B9FFCBA8EF2498597F20508CEDFCC</t>
+  </si>
+  <si>
+    <t> juno1c6wehncdesdssn07azhdwhu3sa0vxc63xalx8gplaxuk3kx88hfsaqrcna</t>
+  </si>
+  <si>
+    <t>ibc/B9EB934D0B4A7BC03D856DA02734D74BD06B4D8955C30274AF6997B117570B4C</t>
+  </si>
+  <si>
+    <t>stars12a0zxmz67vzdvjkt9l0a0ajtj5wvrn034ddfr4wyl8xpurufy8zqnpfmek</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; s --(1)--&gt; j --(1)--&gt; u --(1)--&gt; o --(1)--&gt; s --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>juno16hjuvlufsy625ufs5rxpfu623fknymfw5m2u67t42d2nhd8w94kqraduzk</t>
+  </si>
+  <si>
+    <t>ibc/A40E2545748267BA3C5A7E6F7320352EA9B251A868095A31D1A89A7E2714754E</t>
+  </si>
+  <si>
+    <t>ibc/A96EBA7A6CD3C2725158BAD451F3EF28BBAAE05ADEF2D8BE894DAC86D08E3FD2</t>
+  </si>
+  <si>
+    <t>stars1ted8z7938psc3079jgznr8u405zlseupf39s26kjntyd77g2ehps02jwwm</t>
+  </si>
+  <si>
+    <t>ibc/4606E4EE966207CEEC6C0E77EAC6A9DC9AA843E69883EF821D9D0DE0AE921FB1</t>
+  </si>
+  <si>
+    <t>ibc/0C75E438ABAA09F9C00B4070CB6D3B74BD637523C882AE6D2731D4985EF25370</t>
+  </si>
+  <si>
+    <t>i --(1)--&gt; o --(1)--&gt; s --(1)--&gt; u --(1)--&gt; o --(1)--&gt; j --(1)--&gt; i</t>
+  </si>
+  <si>
+    <t>stars1dhwwzmf356tlsmlvn9dz79h9m55pj2zllht4r79nvaa6g0vusd4shnlu6u</t>
+  </si>
+  <si>
+    <t>ibc/C587232524489D9AA5D1F0020EF67D0F7970760DD53E6764B2DDA481961716B2</t>
+  </si>
+  <si>
+    <t>ibc/899170D90714AAE18489D161466276883763AA4265E8512CD020960DF03B2C30</t>
+  </si>
+  <si>
+    <t>juno1ccltw60vrs89yer3a3y8ymcma353v62k5am3gujvj632dtjgefxsf2g56x</t>
+  </si>
+  <si>
+    <t>ibc/9EF73C7090F618328F37F87ADB2A0B6B48930CCB594B538AE8E0E3B0FDA45DC0</t>
+  </si>
+  <si>
+    <t>93404E5DF495992FB2E66B06055F23F5C84DDA10E2E4DB673B1C9DCEDB6D8C40</t>
+  </si>
+  <si>
+    <t>A55B76A885C9A16E28ACDB1F491C1F62AA30BF5576854FE4D2492FFE4D489CA4</t>
+  </si>
+  <si>
+    <t>EB289548671DF278426A92794C914247A81629A1E60C69FCAAF64AE935D16C27</t>
+  </si>
+  <si>
+    <t>446D0AB77760110606027CE7826783237406F1CC67BF88056F15510409EB93A7</t>
+  </si>
+  <si>
+    <t>9930B9D512E5119F874671B24C640128B1F166613747562B73F6FBB46AA90B70</t>
+  </si>
+  <si>
+    <t>E7C25502A33951F9725C5C5CA1A7342BE9BB12CB7445D8B5546A476CABE2C0C0</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>5CB0BAE632DAE7F0EEC724EDD71D9D2F84783EF7198FA6AE999B56068FF4E4A2</t>
+  </si>
+  <si>
+    <t>B2292906645D0F8725354BC43F06A82097DAD0272AAE5C919B18317000C933B1</t>
+  </si>
+  <si>
+    <t>C828BA261BBA2BF6F89529398CE096118AB8B162BF997A3E496E1FBD9AA71E7A</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>FAD3BCEBD01B5F93AAFA4297C1E4AD13B39C9CE31D2B72F41C85D0DD878ABE8C</t>
+  </si>
+  <si>
+    <t>6279D5FAC9C114E4B8A38370CF0E698E5E83861CF664103140B45768E6BD38D2</t>
+  </si>
+  <si>
+    <t>CDF90E2ABD7C8772BC24E0B67A2F8B7CD7CD623F1A965C210A98B1EF907D138F</t>
+  </si>
+  <si>
+    <t>A7EE7466BE48D592F7663F10C47C4AC0BD7E9BC754959856527447E8F2B1B550</t>
+  </si>
+  <si>
+    <t>B6B295ABF10975668768FB249E8A6370C3BE456E25A0BBD3237E4012F2DCA771</t>
+  </si>
+  <si>
+    <t>6D2C97E2F77F5A3B51867B5DA12EF6425760F3C78ABDE3A1FFB514BACE253DA9</t>
+  </si>
+  <si>
+    <t>DEE62DABE4B4BD187F2B97370C96B156098BE2BAD80A200A0E605CA991BD7FF3</t>
+  </si>
+  <si>
+    <t>gonDenomb4</t>
+  </si>
+  <si>
+    <t>nftIdb4</t>
+  </si>
+  <si>
+    <t>E98FE3AC1D07DBF3FE9290582FF0EBA066258454F5BE91F04B17518FD3394D92</t>
+  </si>
+  <si>
+    <t>7DE7A85BC2EF7C29B4283893ECF6232147874F905E8D8D723C23697BEC51507A</t>
+  </si>
+  <si>
+    <t>4E432F48C1A1B221A821DA71B4AAE8A9987CCB3726CCEE2F389CC89F9CBA00DC</t>
+  </si>
+  <si>
+    <t>EF4B49154EF64F667FCDEA691837F22EB218D9FEA4E70BC749857489CC16E816</t>
+  </si>
+  <si>
+    <t>gonDenomc1</t>
+  </si>
+  <si>
+    <t>nftIdc1</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>F6904B44BAFFEA85F8CD90D79B83225DAC2EBA56C91AD5D38758C4B88EF2FA4D</t>
+  </si>
+  <si>
+    <t>19507C8AD42330C4717A8BFADF5131D1511F9E2C18003F4D45CA781FA82A8E1B</t>
+  </si>
+  <si>
+    <t>EACF70DD4AB94F29352D70C4D04E01B86CC0383954C34EF6009BF9161EA4EA54</t>
+  </si>
+  <si>
+    <t>5A7131ACC111C622D1AD052B71C181DB63F07D5765F0FB42D94B96C89BF021E2</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>82819059D29E98D7BCAFCBF78DEC3CD53ADE4A76AB291B7F8C05B77FCA2A9BCF</t>
+  </si>
+  <si>
+    <t>8C43AB234C807A61127710531DE3B21CFEFF848FE434806BF9D9A3CFF644AB58</t>
+  </si>
+  <si>
+    <t>0236971A3B34ED5A630D98AB9A92DDB1EAE8F5A1F34ECEC1A17AF3150F4153BC</t>
+  </si>
+  <si>
+    <t>900DCD435A95B82ADCA2DA8D3640E2BCAE9F2A3535D546A0FF6762845A1EF070</t>
+  </si>
+  <si>
+    <t>B1BBE98B2D5A2B0E87361AD4696AA07E26FF97D5674AE6FB7E5F5851DE41C6B2</t>
+  </si>
+  <si>
+    <t>313E77E7D7A19A0F3A304E9D1432F8A5B4969D6DCDF8C1078E61D829733FCE57</t>
+  </si>
+  <si>
+    <t>gonDenomc3</t>
+  </si>
+  <si>
+    <t>nftIdc3</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>E2A5347E7FFD8260E2F0AE54AE495527B0EFB4F91C00CD1C352B1C7FE6791796</t>
+  </si>
+  <si>
+    <t>026A8709EC869CDB1627AB5A1B74CCA7EC57D442A540AD232747A0D03A3F884E</t>
+  </si>
+  <si>
+    <t>2483DCD12807FE86D44B65F2B6EE8FF0575096B78F0CD83C758D19C705F4EEEB</t>
+  </si>
+  <si>
+    <t>26D75F551C86009A52A4CD94789E40B914C8C2F60B7B610C9799161F86478A54</t>
+  </si>
+  <si>
+    <t>7CC15F470633E8254D603E98D86C352D78E2D77FD3D84BA85C149142DFEBF36A</t>
+  </si>
+  <si>
+    <t>9A580F7BA6830B8B5F70BDA33B4396B127A90963B2EACA51AFCB38273D3ACA80</t>
   </si>
   <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
@@ -171,12 +405,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -194,6 +428,42 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF6E6B7B"/>
+      <name val="Helvetica"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFB4B7BD"/>
+      <name val="Helvetica"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1A202C"/>
+      <name val="Helvetica"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8.25"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC9D1D9"/>
+      <name val="Helvetica"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -217,6 +487,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -225,8 +503,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -240,18 +525,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -263,24 +548,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -296,21 +587,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,29 +618,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -375,43 +645,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,133 +795,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,42 +875,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -661,16 +905,42 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -678,157 +948,163 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1225,7 +1501,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -1265,25 +1541,25 @@
       </c>
     </row>
     <row r="2" ht="12.75" spans="1:8">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="12" t="s">
         <v>14</v>
       </c>
       <c r="H2" t="s">
@@ -1300,15 +1576,16 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="60.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="42.4017857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1316,15 +1593,42 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" ht="13.2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" ht="13.2" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1337,15 +1641,15 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="55.0625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1353,15 +1657,42 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" ht="13.2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" ht="13.2" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" ht="13.2" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" ht="13.2" spans="1:2">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1374,15 +1705,15 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="65.1785714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1390,15 +1721,58 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" ht="13.2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" ht="13.2" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" ht="13.2" spans="1:2">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" ht="13.2" spans="1:2">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" ht="13.2" spans="1:2">
+      <c r="A6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" ht="13.2" spans="1:2">
+      <c r="A7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1411,15 +1785,15 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="77.0714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1427,15 +1801,58 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" ht="13.2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" ht="13.2" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" ht="13.2" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" ht="13.2" spans="1:2">
+      <c r="A5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" ht="13.2" spans="1:2">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" ht="13.2" spans="1:2">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1448,15 +1865,15 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="63.6875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1464,25 +1881,39 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" ht="13.2" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" ht="13.2" spans="1:1">
-      <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1495,15 +1926,15 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="34.5267857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1511,25 +1942,39 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="13.2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" ht="13.2" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" ht="13.2" spans="1:1">
-      <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>75</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1542,15 +1987,15 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="28.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1558,25 +2003,39 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" ht="13.2" spans="1:1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" ht="13.2" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" ht="13.2" spans="1:1">
+        <v>82</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" ht="13.2" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>83</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1589,15 +2048,15 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="46.2767857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1605,25 +2064,67 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" ht="13.2" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" ht="13.2" spans="1:1">
-      <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" ht="12.8" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" ht="12.8" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" ht="12.8" spans="1:4">
+      <c r="A9" s="4"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" ht="12.8" spans="1:3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1636,15 +2137,15 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="57.4464285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1652,25 +2153,63 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" ht="13.2" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" ht="13.2" spans="1:1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" ht="12.8" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" ht="12.8" spans="1:3">
+      <c r="A3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" ht="13.2" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>93</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1683,15 +2222,15 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B18" sqref="A17:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="56.9910714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1699,25 +2238,52 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" ht="13.2" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" ht="13.2" spans="1:1">
-      <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1730,13 +2296,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="2" width="17.8571428571429" customWidth="1"/>
   </cols>
@@ -1755,6 +2321,14 @@
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1767,15 +2341,15 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B18" sqref="A17:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="40.7767857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1783,25 +2357,68 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" ht="13.2" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" ht="13.2" spans="1:1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" ht="13.2" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>105</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1814,15 +2431,15 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="48.6607142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -1830,25 +2447,68 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
+      <c r="A2" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" ht="13.2" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" ht="13.2" spans="1:1">
-      <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1876,12 +2536,12 @@
     </row>
     <row r="2" ht="16.35" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" ht="13.2" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1912,12 +2572,12 @@
     </row>
     <row r="2" ht="13.2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" ht="13.2" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1948,12 +2608,12 @@
     </row>
     <row r="2" ht="13.2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" ht="13.2" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1984,12 +2644,12 @@
     </row>
     <row r="2" ht="13.2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" ht="13.2" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2005,13 +2665,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="61.6071428571429" customWidth="1"/>
     <col min="2" max="2" width="17.8571428571429" customWidth="1"/>
@@ -2026,29 +2686,40 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="13.2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" ht="13.2" spans="1:3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2081,24 +2752,24 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="13.2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" ht="13.2" spans="2:2">
@@ -2134,24 +2805,24 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="13.2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2184,24 +2855,24 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2216,8 +2887,8 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2236,24 +2907,24 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2266,15 +2937,16 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="60.2678571428571" customWidth="1"/>
+    <col min="3" max="3" width="33.6339285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -2282,16 +2954,41 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" ht="12.8" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" ht="12.8" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" ht="12.8" spans="1:1">
+      <c r="A5" s="7"/>
+    </row>
+    <row r="6" ht="12.8" spans="1:1">
+      <c r="A6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2303,15 +3000,16 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="12" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="55.3571428571429" customWidth="1"/>
+    <col min="3" max="3" width="35.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -2319,15 +3017,34 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" ht="13.2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" ht="13.2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" ht="13.2" spans="1:2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" ht="13.2" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>